<commit_message>
AscendingSupport is now the default sorting strategy
</commit_message>
<xml_diff>
--- a/MED/Project/Documentation/results/results.xlsx
+++ b/MED/Project/Documentation/results/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="car" sheetId="1" r:id="rId1"/>
@@ -483,11 +483,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="95074176"/>
-        <c:axId val="95084544"/>
+        <c:axId val="85309312"/>
+        <c:axId val="85319680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95074176"/>
+        <c:axId val="85309312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -521,7 +521,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95084544"/>
+        <c:crossAx val="85319680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -529,7 +529,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95084544"/>
+        <c:axId val="85319680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.19000000000000003"/>
@@ -561,7 +561,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95074176"/>
+        <c:crossAx val="85309312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -857,11 +857,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="95131520"/>
-        <c:axId val="95137792"/>
+        <c:axId val="85432192"/>
+        <c:axId val="85438464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95131520"/>
+        <c:axId val="85432192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -895,7 +895,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95137792"/>
+        <c:crossAx val="85438464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -903,7 +903,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95137792"/>
+        <c:axId val="85438464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.22000000000000003"/>
@@ -935,7 +935,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95131520"/>
+        <c:crossAx val="85432192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -987,7 +987,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1357,11 +1356,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="96651520"/>
-        <c:axId val="96670080"/>
+        <c:axId val="85903616"/>
+        <c:axId val="86184320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96651520"/>
+        <c:axId val="85903616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1388,14 +1387,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96670080"/>
+        <c:crossAx val="86184320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1403,7 +1401,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96670080"/>
+        <c:axId val="86184320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="50"/>
@@ -1428,21 +1426,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96651520"/>
+        <c:crossAx val="85903616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1487,7 +1483,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1857,11 +1852,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="96708864"/>
-        <c:axId val="96711040"/>
+        <c:axId val="86223104"/>
+        <c:axId val="86225280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96708864"/>
+        <c:axId val="86223104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1888,14 +1883,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96711040"/>
+        <c:crossAx val="86225280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1903,7 +1897,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96711040"/>
+        <c:axId val="86225280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="170"/>
@@ -1928,21 +1922,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96708864"/>
+        <c:crossAx val="86223104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1987,7 +1979,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2231,11 +2222,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="96436608"/>
-        <c:axId val="96438528"/>
+        <c:axId val="86868352"/>
+        <c:axId val="86870272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96436608"/>
+        <c:axId val="86868352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2262,14 +2253,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96438528"/>
+        <c:crossAx val="86870272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2277,7 +2267,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96438528"/>
+        <c:axId val="86870272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.2"/>
@@ -2302,21 +2292,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96436608"/>
+        <c:crossAx val="86868352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2361,7 +2349,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2605,11 +2592,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="96469760"/>
-        <c:axId val="96471680"/>
+        <c:axId val="89260800"/>
+        <c:axId val="89262720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96469760"/>
+        <c:axId val="89260800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2636,14 +2623,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96471680"/>
+        <c:crossAx val="89262720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2651,7 +2637,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96471680"/>
+        <c:axId val="89262720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.9000000000000001"/>
@@ -2676,21 +2662,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96469760"/>
+        <c:crossAx val="89260800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2925,11 +2909,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="96559872"/>
-        <c:axId val="96561792"/>
+        <c:axId val="89023232"/>
+        <c:axId val="89025152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96559872"/>
+        <c:axId val="89023232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2963,7 +2947,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96561792"/>
+        <c:crossAx val="89025152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2971,7 +2955,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96561792"/>
+        <c:axId val="89025152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="170"/>
@@ -3003,7 +2987,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96559872"/>
+        <c:crossAx val="89023232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3245,11 +3229,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="96582272"/>
-        <c:axId val="102306560"/>
+        <c:axId val="89046016"/>
+        <c:axId val="89130112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96582272"/>
+        <c:axId val="89046016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3283,7 +3267,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102306560"/>
+        <c:crossAx val="89130112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3291,7 +3275,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="102306560"/>
+        <c:axId val="89130112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="360"/>
@@ -3323,7 +3307,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96582272"/>
+        <c:crossAx val="89046016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3908,7 +3892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4921,7 +4905,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>